<commit_message>
add * filter to excels
</commit_message>
<xml_diff>
--- a/src/excels/immune/merged_top_genes.xlsx
+++ b/src/excels/immune/merged_top_genes.xlsx
@@ -1273,7 +1273,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ccl3</t>
+          <t>Ccl3*</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1288,7 +1288,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Atf3</t>
+          <t>Atf3*</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1303,7 +1303,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cd83</t>
+          <t>Cd83*</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1318,7 +1318,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fam214b</t>
+          <t>Fam214b*</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1333,7 +1333,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Relb</t>
+          <t>Relb*</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1348,7 +1348,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Gfap</t>
+          <t>Gfap*</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1363,7 +1363,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Uvssa</t>
+          <t>Uvssa*</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1378,7 +1378,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cracr2a</t>
+          <t>Cracr2a*</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1393,7 +1393,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Coro1c</t>
+          <t>Coro1c*</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1408,7 +1408,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chtop</t>
+          <t>Chtop*</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2002,7 +2002,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ccdc88c</t>
+          <t>Ccdc88c*</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2017,7 +2017,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Atp8b4</t>
+          <t>Atp8b4*</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2032,7 +2032,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fau</t>
+          <t>Fau*</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2047,7 +2047,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mctp2</t>
+          <t>Mctp2*</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2062,7 +2062,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Rps14</t>
+          <t>Rps14*</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2077,7 +2077,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lrrc8c</t>
+          <t>Lrrc8c*</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2092,7 +2092,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tpt1</t>
+          <t>Tpt1*</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2107,7 +2107,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dach1</t>
+          <t>Dach1*</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2122,7 +2122,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Atp1b3</t>
+          <t>Atp1b3*</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2137,7 +2137,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>H2-K1</t>
+          <t>H2-K1*</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2152,7 +2152,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Agfg1</t>
+          <t>Agfg1*</t>
         </is>
       </c>
       <c r="B13" t="n">

</xml_diff>